<commit_message>
Update 02 Software-Projekt Tätigkeitsdokumentation.xlsx
</commit_message>
<xml_diff>
--- a/meta/dudpy-planning/02 Software-Projekt Tätigkeitsdokumentation.xlsx
+++ b/meta/dudpy-planning/02 Software-Projekt Tätigkeitsdokumentation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA221F7-F0B1-4409-8053-CFFCF31AFD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB59F1E-906C-4448-A436-AF144543F9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2445" yWindow="1785" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tätigkeitsdokumentation" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="67">
   <si>
     <t>Datei</t>
   </si>
@@ -247,6 +247,18 @@
   </si>
   <si>
     <t>comments 100%</t>
+  </si>
+  <si>
+    <t>Smaller changes</t>
+  </si>
+  <si>
+    <t>compile.bat</t>
+  </si>
+  <si>
+    <t>pyautoinst-config.json</t>
+  </si>
+  <si>
+    <t>Had some edge cases</t>
   </si>
 </sst>
 </file>
@@ -471,14 +483,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -820,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,12 +849,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14" t="s">
         <v>15</v>
@@ -875,7 +887,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -913,7 +925,7 @@
       <c r="E4" s="9">
         <v>2</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="16" t="s">
         <v>32</v>
       </c>
       <c r="G4" s="10" t="s">
@@ -953,13 +965,13 @@
       <c r="C6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>374</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="16">
         <v>2</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="16" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="10" t="s">
@@ -967,7 +979,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -976,13 +988,13 @@
       <c r="C7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <v>3</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="16">
         <v>1</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="16" t="s">
         <v>21</v>
       </c>
       <c r="G7" s="10" t="s">
@@ -999,13 +1011,13 @@
       <c r="C8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <v>4</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="16">
         <v>1</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="16" t="s">
         <v>32</v>
       </c>
       <c r="G8" s="10" t="s">
@@ -1013,7 +1025,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1022,13 +1034,13 @@
       <c r="C9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="16">
         <v>16</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="16">
         <v>1</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="16" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="10" t="s">
@@ -1045,13 +1057,13 @@
       <c r="C10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="16">
         <v>32</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="16">
         <v>1</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="16" t="s">
         <v>27</v>
       </c>
       <c r="G10" s="10" t="s">
@@ -1059,7 +1071,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1068,13 +1080,13 @@
       <c r="C11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="16">
         <v>70</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="16">
         <v>1</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="16" t="s">
         <v>21</v>
       </c>
       <c r="G11" s="10" t="s">
@@ -1091,13 +1103,13 @@
       <c r="C12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="16">
         <v>23</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="16">
         <v>1</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="16" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="10" t="s">
@@ -1114,13 +1126,13 @@
       <c r="C13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="16">
         <v>11</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="16">
         <v>1</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="16" t="s">
         <v>21</v>
       </c>
       <c r="G13" s="10" t="s">
@@ -1137,13 +1149,13 @@
       <c r="C14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="16">
         <v>6</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="16">
         <v>1</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="16" t="s">
         <v>21</v>
       </c>
       <c r="G14" s="10" t="s">
@@ -1151,7 +1163,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1163,7 +1175,7 @@
       <c r="D15" s="9">
         <v>32</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="16">
         <v>2</v>
       </c>
       <c r="F15" t="s">
@@ -1172,7 +1184,7 @@
       <c r="G15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="16" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1186,10 +1198,10 @@
       <c r="C16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="16">
         <v>23</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="16">
         <v>2</v>
       </c>
       <c r="F16" t="s">
@@ -1198,7 +1210,7 @@
       <c r="G16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="16" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1212,10 +1224,10 @@
       <c r="C17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="16">
         <v>25</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="16">
         <v>2</v>
       </c>
       <c r="F17" t="s">
@@ -1224,12 +1236,12 @@
       <c r="G17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="16" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -1241,10 +1253,10 @@
       <c r="D18" s="9">
         <v>58</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="16">
         <v>2</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="16" t="s">
         <v>21</v>
       </c>
       <c r="G18" s="10" t="s">
@@ -1264,7 +1276,7 @@
       <c r="D19" s="9">
         <v>17</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="16">
         <v>2</v>
       </c>
       <c r="F19" t="s">
@@ -1287,10 +1299,10 @@
       <c r="D20" s="9">
         <v>14</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="16">
         <v>2</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="16" t="s">
         <v>21</v>
       </c>
       <c r="G20" s="10" t="s">
@@ -1310,10 +1322,10 @@
       <c r="D21" s="9">
         <v>32</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="16">
         <v>2</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="16" t="s">
         <v>21</v>
       </c>
       <c r="G21" s="10" t="s">
@@ -1321,19 +1333,19 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="15" t="s">
         <v>53</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="16" t="s">
         <v>54</v>
       </c>
       <c r="D22" s="9">
         <v>0</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="16">
         <v>1</v>
       </c>
       <c r="F22" t="s">
@@ -1350,13 +1362,13 @@
       <c r="B23" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="16" t="s">
         <v>54</v>
       </c>
       <c r="D23" s="9">
         <v>0</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="16">
         <v>1</v>
       </c>
       <c r="F23" t="s">
@@ -1373,13 +1385,13 @@
       <c r="B24" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="16">
         <v>0</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="16">
         <v>1</v>
       </c>
       <c r="F24" t="s">
@@ -1396,13 +1408,13 @@
       <c r="B25" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="16" t="s">
         <v>55</v>
       </c>
       <c r="D25" s="9">
         <v>0</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="16">
         <v>1</v>
       </c>
       <c r="F25" t="s">
@@ -1419,13 +1431,13 @@
       <c r="B26" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="16" t="s">
         <v>55</v>
       </c>
       <c r="D26" s="9">
         <v>0</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="16">
         <v>1</v>
       </c>
       <c r="F26" t="s">
@@ -1442,13 +1454,13 @@
       <c r="B27" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="16">
         <v>0</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27" s="16">
         <v>1</v>
       </c>
       <c r="F27" t="s">
@@ -1459,22 +1471,22 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="15" t="s">
         <v>56</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="16">
         <v>-20</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E28" s="16">
         <v>1</v>
       </c>
-      <c r="F28" s="18" t="s">
+      <c r="F28" s="16" t="s">
         <v>27</v>
       </c>
       <c r="G28" s="10" t="s">
@@ -1482,19 +1494,19 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="15" t="s">
         <v>58</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="16">
         <v>0</v>
       </c>
-      <c r="E29" s="18">
+      <c r="E29" s="16">
         <v>1</v>
       </c>
       <c r="F29" t="s">
@@ -1511,16 +1523,16 @@
       <c r="B30" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="16">
         <v>6</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E30" s="16">
         <v>1</v>
       </c>
-      <c r="F30" s="18" t="s">
+      <c r="F30" s="16" t="s">
         <v>62</v>
       </c>
       <c r="G30" s="10" t="s">
@@ -1528,18 +1540,53 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="G31" s="10"/>
+      <c r="A31" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="16">
+        <v>9</v>
+      </c>
+      <c r="E31" s="16">
+        <v>2</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="G32" s="10"/>
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="16">
+        <v>0</v>
+      </c>
+      <c r="E32" s="16">
+        <v>2</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="8"/>
@@ -1823,9 +1870,10 @@
     <hyperlink ref="A22" r:id="rId7" location="diff-c7cae56b122b1279c1580d7603c1f10ceca6ba3e677310ecf9ece20f250a555f" xr:uid="{81F89C16-0E5C-4949-8A21-59CD9C6E28B3}"/>
     <hyperlink ref="A28" r:id="rId8" location="diff-2e5ad92c43aa96cc3a9cef6c6aec998b216f1379c43b1f651013d25e55989312" xr:uid="{128BC125-D931-4B98-975F-FA8F5618BD0B}"/>
     <hyperlink ref="A29" r:id="rId9" location="diff-b335630551682c19a781afebcf4d07bf978fb1f8ac04c6bf87428ed5106870f5" xr:uid="{FE4659F6-2970-4238-B391-D93626E91E4D}"/>
+    <hyperlink ref="A31" r:id="rId10" xr:uid="{B6E8F3A1-0F2B-4FDE-AFD9-F584E89B35BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Implemented DCGNode and associated serializers
</commit_message>
<xml_diff>
--- a/meta/dudpy-planning/02 Software-Projekt Tätigkeitsdokumentation.xlsx
+++ b/meta/dudpy-planning/02 Software-Projekt Tätigkeitsdokumentation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50CEC51-3071-4AB7-AFE6-127C294018FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11550FF4-3197-42B7-B632-E6059383E4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28065" yWindow="2595" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tätigkeitsdokumentation" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="93">
   <si>
     <t>Datei</t>
   </si>
@@ -301,6 +301,42 @@
   </si>
   <si>
     <t>moved sidebar to the left</t>
+  </si>
+  <si>
+    <t>implemented proper file ...</t>
+  </si>
+  <si>
+    <t>implemented basic seri...</t>
+  </si>
+  <si>
+    <t>src\dc\displayManager (temp)</t>
+  </si>
+  <si>
+    <t>renamed Position...</t>
+  </si>
+  <si>
+    <t>setter</t>
+  </si>
+  <si>
+    <t>src\dc\core\modules\state.py</t>
+  </si>
+  <si>
+    <t>added getter ...</t>
+  </si>
+  <si>
+    <t>src\dc\core\dfa\DFAstate.py</t>
+  </si>
+  <si>
+    <t>added serialisation ...</t>
+  </si>
+  <si>
+    <t>updated serialisation ...</t>
+  </si>
+  <si>
+    <t>changed to pickle</t>
+  </si>
+  <si>
+    <t>src\dc\serializer.py (temp)</t>
   </si>
 </sst>
 </file>
@@ -501,7 +537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -527,6 +563,8 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -875,7 +913,7 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,12 +929,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14" t="s">
         <v>15</v>
@@ -1815,39 +1853,116 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="8"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="G41" s="10"/>
+      <c r="A41" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="16">
+        <v>31</v>
+      </c>
+      <c r="E41" s="16">
+        <v>2</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="8"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="G42" s="10"/>
+      <c r="A42" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" s="16">
+        <v>4</v>
+      </c>
+      <c r="E42" s="16">
+        <v>1</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="8"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="G43" s="10"/>
+      <c r="A43" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" s="9">
+        <v>24</v>
+      </c>
+      <c r="E43" s="16">
+        <v>2</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="8"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="G44" s="10"/>
+      <c r="A44" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="16">
+        <v>51</v>
+      </c>
+      <c r="E44" s="16">
+        <v>1</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="8"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="G45" s="10"/>
+      <c r="B45" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" s="9">
+        <v>151</v>
+      </c>
+      <c r="E45" s="9">
+        <v>2</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" s="8"/>
@@ -2045,9 +2160,13 @@
     <hyperlink ref="A36" r:id="rId12" location="diff-8c86fe1dccd9fa33874649ecdb94b100ba17b9a344f0b64b343c93565a1d1b61" xr:uid="{55C9BCC4-9D86-4C8E-A405-C75CBCA37978}"/>
     <hyperlink ref="A37" r:id="rId13" location="diff-8c86fe1dccd9fa33874649ecdb94b100ba17b9a344f0b64b343c93565a1d1b61" xr:uid="{258E7277-F4C4-47A0-9C41-C8812B495DAF}"/>
     <hyperlink ref="A38" r:id="rId14" location="diff-24a3fe5c783755412cb9de83238b4dfd0699345bf50dcadc3ec23c6749361592" xr:uid="{BFD3B569-D5C6-422C-84E1-7F4AA8A68744}"/>
+    <hyperlink ref="A41" r:id="rId15" location="diff-3d2678f49f03c05fe20e8802e3516e3d8c9dd5bce813e0845552a9d793e7593d" xr:uid="{123DAC12-35F9-4441-81E3-D6B431C3BF80}"/>
+    <hyperlink ref="A42" r:id="rId16" location="diff-7193f7df8c6f35c6f42d6f9db6deb3bf3d1a1000927552b84c901eca5b9b37e0" xr:uid="{D797A1C0-AD1D-44EC-9523-DCE63CBC652C}"/>
+    <hyperlink ref="A43" r:id="rId17" location="diff-40c55730b9514e3da9867e2fbb856d7a9506c78cedd35f9c83955a83340286ad" xr:uid="{CFBAD435-50E3-49D4-9579-5F6E11506405}"/>
+    <hyperlink ref="A44" r:id="rId18" location="diff-637e49ef799bb51094751e67276f1dfeaeb31048cd7e0de7c90fef139d184c88" xr:uid="{8EBCA02C-10BC-423A-B06E-3F3D019D27BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>